<commit_message>
Getting stack overflow on Problem #14.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\euler2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="24915" windowHeight="12585"/>
   </bookViews>
@@ -698,12 +693,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="162250320"/>
-        <c:axId val="161260672"/>
+        <c:axId val="173048192"/>
+        <c:axId val="173050112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="162250320"/>
+        <c:axId val="173048192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +728,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161260672"/>
+        <c:crossAx val="173050112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -740,7 +736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161260672"/>
+        <c:axId val="173050112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +766,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162250320"/>
+        <c:crossAx val="173048192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -841,26 +837,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1153,11 +1129,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="528552128"/>
-        <c:axId val="528547032"/>
+        <c:axId val="173090688"/>
+        <c:axId val="173092224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="528552128"/>
+        <c:axId val="173090688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528547032"/>
+        <c:crossAx val="173092224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1207,7 +1183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="528547032"/>
+        <c:axId val="173092224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1229,17 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
@@ -1279,26 +1265,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1331,7 +1297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="528552128"/>
+        <c:crossAx val="173090688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2624,7 +2590,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2659,7 +2625,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2870,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update categories to be consistent.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -704,11 +704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="75649024"/>
-        <c:axId val="58119232"/>
+        <c:axId val="39342592"/>
+        <c:axId val="100914240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75649024"/>
+        <c:axId val="39342592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +737,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58119232"/>
+        <c:crossAx val="100914240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -745,7 +745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58119232"/>
+        <c:axId val="100914240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +775,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75649024"/>
+        <c:crossAx val="39342592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -909,7 +909,7 @@
                   <c:v>51.001930713653564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.383390999999996</c:v>
+                  <c:v>28.391290999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,11 +1147,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="75651072"/>
-        <c:axId val="76685888"/>
+        <c:axId val="39344128"/>
+        <c:axId val="40378944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75651072"/>
+        <c:axId val="39344128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76685888"/>
+        <c:crossAx val="40378944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1201,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76685888"/>
+        <c:axId val="40378944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75651072"/>
+        <c:crossAx val="39344128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2855,7 +2855,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3006,7 +3006,7 @@
         <v>3.0529000000000001E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L18" si="2">IF(G4/J4&lt;1,-1*J4/G4,G4/J4)</f>
+        <f t="shared" ref="L4:L19" si="2">IF(G4/J4&lt;1,-1*J4/G4,G4/J4)</f>
         <v>1.7491631594215762</v>
       </c>
     </row>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="P8">
         <f>SUM(J2:J45)</f>
-        <v>23.383390999999996</v>
+        <v>28.391290999999999</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
@@ -3625,6 +3625,13 @@
         <f t="shared" si="4"/>
         <v>25.194070100784302</v>
       </c>
+      <c r="J19">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>1.4350414276123047</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -3683,6 +3690,9 @@
         <f t="shared" si="4"/>
         <v>25.203980207443237</v>
       </c>
+      <c r="J21">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -3712,6 +3722,9 @@
         <f t="shared" si="4"/>
         <v>25.210730314254761</v>
       </c>
+      <c r="J22">
+        <v>8.9999999999999998E-4</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -3740,6 +3753,9 @@
       <c r="H23" s="2">
         <f t="shared" si="4"/>
         <v>29.588560342788696</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>